<commit_message>
Changing squad json serialization to scriptable objects. Editor scripts to allow editing of squad layouts intuitively in the editor. Cleaning up old + unused files. Some project reorganization.
</commit_message>
<xml_diff>
--- a/DesignDocuments/UnitBalanceSpreadsheet.xlsx
+++ b/DesignDocuments/UnitBalanceSpreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ari\Documents\GameDev\DragonFodder\DesignDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{912BF08D-6069-4400-B25F-4ECA4F36D4E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A034393D-B0B8-439D-8962-47CF4728AB2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{50A833F2-5FC8-4F78-AA4C-C0E3D82D8445}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Unit</t>
   </si>
@@ -82,6 +82,12 @@
   </si>
   <si>
     <t>Time Between Attacks</t>
+  </si>
+  <si>
+    <t>Testing results</t>
+  </si>
+  <si>
+    <t>Ghoul</t>
   </si>
 </sst>
 </file>
@@ -487,7 +493,7 @@
   <dimension ref="A1:P33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,13 +507,14 @@
     <col min="8" max="8" width="15.85546875" style="1" customWidth="1"/>
     <col min="9" max="9" width="17.140625" style="1" customWidth="1"/>
     <col min="10" max="10" width="13.42578125" style="1" customWidth="1"/>
-    <col min="11" max="14" width="9.140625" style="1"/>
+    <col min="11" max="11" width="27.42578125" style="1" customWidth="1"/>
+    <col min="12" max="14" width="9.140625" style="1"/>
     <col min="15" max="15" width="24.140625" style="1" customWidth="1"/>
     <col min="16" max="16" width="43.140625" style="1" customWidth="1"/>
     <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -537,6 +544,9 @@
       </c>
       <c r="J1" s="2" t="s">
         <v>4</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -591,7 +601,7 @@
         <v>1</v>
       </c>
       <c r="J3" s="1">
-        <f>D3*F3/10 +G3*I3/100</f>
+        <f t="shared" ref="J3:J33" si="1">D3*F3/10 +G3*I3/100</f>
         <v>1.5</v>
       </c>
     </row>
@@ -600,14 +610,14 @@
         <v>13</v>
       </c>
       <c r="B4" s="1">
-        <v>0.9</v>
+        <v>0.6</v>
       </c>
       <c r="C4" s="1">
         <v>5</v>
       </c>
       <c r="D4" s="1">
         <f t="shared" si="0"/>
-        <v>5.5555555555555554</v>
+        <v>8.3333333333333339</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>14</v>
@@ -616,14 +626,14 @@
         <v>1.5</v>
       </c>
       <c r="G4" s="1">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="I4" s="3">
         <v>1</v>
       </c>
       <c r="J4" s="1">
-        <f t="shared" ref="J3:J33" si="1">D4*F4/10 +G4*I4/50</f>
-        <v>2.0333333333333332</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>6</v>
@@ -633,19 +643,31 @@
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D5" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="A5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="C5" s="1">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" si="0"/>
+        <v>6.666666666666667</v>
       </c>
       <c r="F5" s="1">
         <v>1</v>
       </c>
+      <c r="G5" s="1">
+        <v>80</v>
+      </c>
       <c r="I5" s="3">
         <v>1</v>
       </c>
-      <c r="J5" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="J5" s="1">
+        <f t="shared" si="1"/>
+        <v>1.4666666666666668</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Adding menu in game scenes to return to main menu and quit game. First build (not in repo)!
</commit_message>
<xml_diff>
--- a/DesignDocuments/UnitBalanceSpreadsheet.xlsx
+++ b/DesignDocuments/UnitBalanceSpreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ari\Documents\GameDev\DragonFodder\DesignDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A034393D-B0B8-439D-8962-47CF4728AB2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD0D5C9D-DC6F-4722-9C7D-72A814485E13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{50A833F2-5FC8-4F78-AA4C-C0E3D82D8445}"/>
+    <workbookView xWindow="-12810" yWindow="5355" windowWidth="21600" windowHeight="11385" xr2:uid="{50A833F2-5FC8-4F78-AA4C-C0E3D82D8445}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Unit</t>
   </si>
@@ -88,6 +88,24 @@
   </si>
   <si>
     <t>Ghoul</t>
+  </si>
+  <si>
+    <t>Vampire</t>
+  </si>
+  <si>
+    <t>Zombie</t>
+  </si>
+  <si>
+    <t>Life Steal</t>
+  </si>
+  <si>
+    <t>Stun</t>
+  </si>
+  <si>
+    <t>Mummy</t>
+  </si>
+  <si>
+    <t>Vulnerable</t>
   </si>
 </sst>
 </file>
@@ -493,7 +511,7 @@
   <dimension ref="A1:P33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,67 +597,67 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="C3" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D3" s="1">
         <f t="shared" ref="D3:D33" si="0">C3/B3</f>
-        <v>10</v>
+        <v>8.3333333333333339</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="F3" s="1">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="G3" s="1">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="I3" s="3">
         <v>1</v>
       </c>
       <c r="J3" s="1">
         <f t="shared" ref="J3:J33" si="1">D3*F3/10 +G3*I3/100</f>
-        <v>1.5</v>
+        <v>2</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="C4" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D4" s="1">
-        <f t="shared" si="0"/>
-        <v>8.3333333333333339</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>14</v>
+        <f>C4/B4</f>
+        <v>10</v>
       </c>
       <c r="F4" s="1">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1">
+        <v>50</v>
+      </c>
+      <c r="I4" s="3">
+        <v>1</v>
+      </c>
+      <c r="J4" s="1">
+        <f>D4*F4/10 +G4*I4/100</f>
         <v>1.5</v>
-      </c>
-      <c r="G4" s="1">
-        <v>75</v>
-      </c>
-      <c r="I4" s="3">
-        <v>1</v>
-      </c>
-      <c r="J4" s="1">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -647,14 +665,14 @@
         <v>17</v>
       </c>
       <c r="B5" s="1">
-        <v>1.5</v>
+        <v>0.75</v>
       </c>
       <c r="C5" s="1">
         <v>10</v>
       </c>
       <c r="D5" s="1">
         <f t="shared" si="0"/>
-        <v>6.666666666666667</v>
+        <v>13.333333333333334</v>
       </c>
       <c r="F5" s="1">
         <v>1</v>
@@ -667,55 +685,101 @@
       </c>
       <c r="J5" s="1">
         <f t="shared" si="1"/>
-        <v>1.4666666666666668</v>
+        <v>2.1333333333333337</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D6" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="A6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C6" s="1">
+        <v>10</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
       <c r="F6" s="1">
         <v>1</v>
       </c>
+      <c r="G6" s="1">
+        <v>100</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="I6" s="3">
-        <v>1</v>
-      </c>
-      <c r="J6" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <f>(G6 + D6*0.25*5)/G6</f>
+        <v>1.25</v>
+      </c>
+      <c r="J6" s="1">
+        <f t="shared" si="1"/>
+        <v>3.25</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D7" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="A7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="1">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1">
+        <v>20</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" si="0"/>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="F7" s="1">
-        <v>1</v>
+        <v>1.5</v>
+      </c>
+      <c r="G7" s="1">
+        <v>150</v>
       </c>
       <c r="I7" s="3">
         <v>1</v>
       </c>
-      <c r="J7" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="J7" s="1">
+        <f t="shared" si="1"/>
+        <v>2.5</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D8" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="A8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="1">
+        <v>2</v>
+      </c>
+      <c r="C8" s="1">
+        <v>15</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
+        <v>7.5</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="F8" s="1">
-        <v>1</v>
+        <v>1.25</v>
+      </c>
+      <c r="G8" s="1">
+        <v>200</v>
       </c>
       <c r="I8" s="3">
         <v>1</v>
       </c>
-      <c r="J8" s="1" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="J8" s="1">
+        <f t="shared" si="1"/>
+        <v>2.9375</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>